<commit_message>
Made sure all filepaths worked correctly
</commit_message>
<xml_diff>
--- a/Keele_F_Reed_C-P0/ExcelSheets/VendorList&Inventory.xlsx
+++ b/Keele_F_Reed_C-P0/ExcelSheets/VendorList&Inventory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0-Project\Keele_F_Reed_C-P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0-Project\Keele_F_Reed_C-P0\Keele_F_Reed_C-P0\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957FB830-563F-484E-A3F6-E2A822108B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3941CD6D-375A-4AC8-91DA-98AB39DD482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="1065" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{022B787D-45AC-4743-9C03-998D2CE48FCF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Vendors</t>
   </si>
@@ -109,16 +109,19 @@
     <t>Pencils</t>
   </si>
   <si>
+    <t>MouseTraps</t>
+  </si>
+  <si>
+    <t>Burrito</t>
+  </si>
+  <si>
+    <t>Salsa</t>
+  </si>
+  <si>
+    <t>Powerade</t>
+  </si>
+  <si>
     <t>Pickles</t>
-  </si>
-  <si>
-    <t>MouseTraps</t>
-  </si>
-  <si>
-    <t>Burrito</t>
-  </si>
-  <si>
-    <t>Salsa</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D08D3-1D91-4FD2-BDB6-9D61C099D0F4}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +736,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>52</v>
@@ -744,7 +747,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>16</v>
@@ -755,7 +758,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
         <v>45</v>
@@ -766,13 +769,24 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>12</v>
       </c>
       <c r="C20" s="3">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>